<commit_message>
MAJ tableau des tâches sprint 1
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Documents\travail\EMN\MiniCraft\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16845" windowHeight="3510"/>
   </bookViews>
@@ -12,12 +17,11 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -52,13 +56,10 @@
     <t>Ouvrir une fenêtre avec un monde plat</t>
   </si>
   <si>
-    <t>Montée en compétence sur Jmonkey</t>
-  </si>
-  <si>
-    <t>14H</t>
-  </si>
-  <si>
-    <t>1H</t>
+    <t>Montée en compétence sur Jmonkey &amp; install</t>
+  </si>
+  <si>
+    <t>Création des tâches et graphes agiles</t>
   </si>
 </sst>
 </file>
@@ -441,7 +442,7 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,8 +491,8 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
+      <c r="E5" s="2">
+        <v>13</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
@@ -500,40 +501,48 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E8">
         <f>SUM(E5:E7)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <f>SUM(F5:F7)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de graphe RAF dans Agile.xsl
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -47,9 +47,6 @@
     <t>#2</t>
   </si>
   <si>
-    <t>Avancement %</t>
-  </si>
-  <si>
     <t>#3</t>
   </si>
   <si>
@@ -60,6 +57,15 @@
   </si>
   <si>
     <t>Création des tâches et graphes agiles</t>
+  </si>
+  <si>
+    <t>Reste à faire %</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>RAF</t>
   </si>
 </sst>
 </file>
@@ -150,6 +156,910 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Evalution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> du RAF en % en fonction du sprint</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$12:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="214329344"/>
+        <c:axId val="214328560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="214329344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="214328560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="214328560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="214329344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>210911</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>34698</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>639536</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>110898</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +1364,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -486,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -497,14 +1407,16 @@
       <c r="F5" s="2">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -515,14 +1427,16 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -533,7 +1447,9 @@
       <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E8">
@@ -545,9 +1461,58 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MAJ tâches et avancement
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -50,12 +50,6 @@
     <t>#3</t>
   </si>
   <si>
-    <t>Ouvrir une fenêtre avec un monde plat</t>
-  </si>
-  <si>
-    <t>Montée en compétence sur Jmonkey &amp; install</t>
-  </si>
-  <si>
     <t>Création des tâches et graphes agiles</t>
   </si>
   <si>
@@ -66,6 +60,30 @@
   </si>
   <si>
     <t>RAF</t>
+  </si>
+  <si>
+    <t>Ouvrir une fenêtre avec un monde  16x16 blocs</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Poser des blocs et enlever des blocs</t>
+  </si>
+  <si>
+    <t>Intégration système de collisions (solide)</t>
+  </si>
+  <si>
+    <t>Vue à la première personne + imposer gravité</t>
+  </si>
+  <si>
+    <t>Montée en compétence sur Jmonkey &amp; installation</t>
   </si>
 </sst>
 </file>
@@ -256,7 +274,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$12:$B$16</c:f>
+              <c:f>Feuil1!$M$7:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -280,7 +298,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$12:$C$16</c:f>
+              <c:f>Feuil1!$N$7:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -313,11 +331,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="214329344"/>
-        <c:axId val="214328560"/>
+        <c:axId val="185125384"/>
+        <c:axId val="185126504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="214329344"/>
+        <c:axId val="185125384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +378,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214328560"/>
+        <c:crossAx val="185126504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -368,7 +386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214328560"/>
+        <c:axId val="185126504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,7 +440,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214329344"/>
+        <c:crossAx val="185125384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1031,15 +1049,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>210911</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>34698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>110898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1349,31 +1367,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1391,32 +1409,32 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -1427,16 +1445,20 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="2">
-        <v>100</v>
+      <c r="G6" s="2"/>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1445,67 +1467,104 @@
         <v>2</v>
       </c>
       <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
-        <v>100</v>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <f>SUM(E5:E7)</f>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8">
-        <f>SUM(F5:F7)</f>
-        <v>10</v>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>SUM(E5:E10)</f>
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F5:F10)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="G11">
+        <v>90</v>
+      </c>
+      <c r="M11">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="N11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise en place du dossier assets pour l'assetManager (utile pour les imports multimedias : sons, textures pour cubes, etc...) + ajouter au build path Mise a jour tâches et avancement
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -50,12 +50,6 @@
     <t>#3</t>
   </si>
   <si>
-    <t>Ouvrir une fenêtre avec un monde plat</t>
-  </si>
-  <si>
-    <t>Montée en compétence sur Jmonkey &amp; install</t>
-  </si>
-  <si>
     <t>Création des tâches et graphes agiles</t>
   </si>
   <si>
@@ -66,6 +60,30 @@
   </si>
   <si>
     <t>RAF</t>
+  </si>
+  <si>
+    <t>Ouvrir une fenêtre avec un monde  16x16 blocs</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Poser des blocs et enlever des blocs</t>
+  </si>
+  <si>
+    <t>Intégration système de collisions (solide)</t>
+  </si>
+  <si>
+    <t>Vue à la première personne + imposer gravité</t>
+  </si>
+  <si>
+    <t>Montée en compétence sur Jmonkey &amp; installation</t>
   </si>
 </sst>
 </file>
@@ -256,7 +274,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$12:$B$16</c:f>
+              <c:f>Feuil1!$M$7:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -280,7 +298,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$12:$C$16</c:f>
+              <c:f>Feuil1!$N$7:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -313,11 +331,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="214329344"/>
-        <c:axId val="214328560"/>
+        <c:axId val="185125384"/>
+        <c:axId val="185126504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="214329344"/>
+        <c:axId val="185125384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +378,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214328560"/>
+        <c:crossAx val="185126504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -368,7 +386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214328560"/>
+        <c:axId val="185126504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,7 +440,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214329344"/>
+        <c:crossAx val="185125384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1031,15 +1049,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>210911</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>34698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>110898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1349,31 +1367,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1391,32 +1409,32 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -1427,16 +1445,20 @@
       <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" s="2">
-        <v>100</v>
+      <c r="G6" s="2"/>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1445,67 +1467,104 @@
         <v>2</v>
       </c>
       <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
-        <v>100</v>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <f>SUM(E5:E7)</f>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8">
-        <f>SUM(F5:F7)</f>
-        <v>10</v>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>SUM(E5:E10)</f>
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <f>SUM(F5:F10)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="G11">
+        <v>90</v>
+      </c>
+      <c r="M11">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="N11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MAJ des docs avancement
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16845" windowHeight="3510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Durée estimée (h)</t>
   </si>
   <si>
-    <t>Durée restante</t>
-  </si>
-  <si>
     <t>#1</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>Reste à faire %</t>
   </si>
   <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>RAF</t>
-  </si>
-  <si>
     <t>Ouvrir une fenêtre avec un monde  16x16 blocs</t>
   </si>
   <si>
@@ -84,6 +75,15 @@
   </si>
   <si>
     <t>Montée en compétence sur Jmonkey &amp; installation</t>
+  </si>
+  <si>
+    <t>Durée restante (h)</t>
+  </si>
+  <si>
+    <t>Mise en place du dépôt Git &amp; maîtrise de cet outil</t>
+  </si>
+  <si>
+    <t>RELEASE</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -144,11 +144,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -157,6 +175,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -215,9 +245,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> du RAF en % en fonction du sprint</a:t>
+              <a:t> du RAF pendant le sprint 1 (en % )</a:t>
             </a:r>
-            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -258,12 +287,35 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$N$6:$N$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29/05/2013</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -272,33 +324,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Feuil1!$M$7:$M$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$N$7:$N$11</c:f>
+              <c:f>Feuil1!$M$6:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -306,16 +334,16 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -331,54 +359,52 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="185125384"/>
-        <c:axId val="185126504"/>
+        <c:axId val="187956240"/>
+        <c:axId val="187963184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185125384"/>
+        <c:axId val="187956240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="185126504"/>
+        <c:crossAx val="187963184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -386,7 +412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185126504"/>
+        <c:axId val="187963184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,6 +432,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>RAF</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> en %</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -440,7 +527,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185125384"/>
+        <c:crossAx val="187956240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1049,16 +1136,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>210911</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>34698</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57645</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>72798</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>110898</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>486270</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>148998</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1367,29 +1454,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N11"/>
+  <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G2" s="3" t="s">
-        <v>10</v>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -1404,85 +1501,139 @@
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="6">
+        <v>41415</v>
+      </c>
+      <c r="G4" s="6">
+        <v>41418</v>
+      </c>
+      <c r="H4" s="6">
+        <v>41421</v>
+      </c>
+      <c r="I4" s="6">
+        <v>41422</v>
+      </c>
+      <c r="J4" s="6">
+        <v>41423</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
-        <v>100</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="2">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="M6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" t="s">
-        <v>12</v>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>100</v>
+      </c>
+      <c r="N6" s="6">
+        <v>41415</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>100</v>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>90</v>
+      </c>
+      <c r="N7" s="6">
+        <v>41418</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1493,23 +1644,37 @@
       <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="M8">
+      <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="N8">
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
         <v>80</v>
+      </c>
+      <c r="N8" s="6">
+        <v>41421</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -1517,58 +1682,138 @@
       <c r="F9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
         <v>60</v>
+      </c>
+      <c r="N9" s="6">
+        <v>41422</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <v>5</v>
       </c>
       <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2">
         <v>2</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="M10">
-        <v>4</v>
-      </c>
-      <c r="N10">
-        <v>30</v>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>55</v>
+      </c>
+      <c r="N10" s="6">
+        <v>41423</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <f>SUM(E5:E10)</f>
-        <v>24</v>
-      </c>
-      <c r="F11">
-        <f>SUM(F5:F10)</f>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G11">
-        <v>90</v>
-      </c>
-      <c r="M11">
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="N11">
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>50</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>SUM(E6:E11)</f>
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <f>SUM(F6:F11)</f>
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <f>SUM(G6:G11)</f>
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <f>SUM(H6:H11)</f>
+        <v>16</v>
+      </c>
+      <c r="I12">
+        <f>SUM(I6:I11)</f>
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <f>SUM(J6:J11)</f>
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <f>SUM(K6:K11)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:K3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
MAJ doc avancement et graphe SCRUM
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -12,16 +12,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$A$2:$J$33</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ITERATION 1</t>
   </si>
@@ -83,14 +86,14 @@
     <t>Mise en place du dépôt Git &amp; maîtrise de cet outil</t>
   </si>
   <si>
-    <t>RELEASE</t>
+    <t>#7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +103,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,18 +163,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -180,18 +182,17 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -291,7 +292,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$N$6:$N$10</c:f>
+              <c:f>Sprint1!$J$20:$J$24</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -326,24 +327,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$M$6:$M$10</c:f>
+              <c:f>Sprint1!$I$20:$I$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>0.93103448275862066</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>0.7931034482758621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
+                  <c:v>0.55172413793103448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>0.34482758620689657</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>0.20689655172413793</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,17 +360,42 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="187956240"/>
-        <c:axId val="187963184"/>
+        <c:axId val="180812224"/>
+        <c:axId val="180814224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="187956240"/>
+        <c:axId val="180812224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -404,7 +430,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187963184"/>
+        <c:crossAx val="180814224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -412,7 +438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187963184"/>
+        <c:axId val="180814224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,7 +519,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -527,7 +553,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187956240"/>
+        <c:crossAx val="180812224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,16 +1162,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57645</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>72798</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>213509</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>486270</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>148998</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1454,41 +1480,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N12"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B3:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9"/>
-      <c r="M3" s="2"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1516,13 +1540,11 @@
       <c r="J4" s="6">
         <v>41423</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
+    <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1547,14 +1569,10 @@
       <c r="J5" s="2">
         <v>0</v>
       </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -1580,19 +1598,10 @@
       <c r="J6" s="2">
         <v>2</v>
       </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>100</v>
-      </c>
-      <c r="N6" s="6">
-        <v>41415</v>
-      </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -1618,19 +1627,10 @@
       <c r="J7" s="2">
         <v>0</v>
       </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>90</v>
-      </c>
-      <c r="N7" s="6">
-        <v>41418</v>
-      </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -1656,19 +1656,10 @@
       <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>80</v>
-      </c>
-      <c r="N8" s="6">
-        <v>41421</v>
-      </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1694,19 +1685,10 @@
       <c r="J9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>60</v>
-      </c>
-      <c r="N9" s="6">
-        <v>41422</v>
-      </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1732,19 +1714,10 @@
       <c r="J10" s="2">
         <v>2</v>
       </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>55</v>
-      </c>
-      <c r="N10" s="6">
-        <v>41423</v>
-      </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1770,52 +1743,100 @@
       <c r="J11" s="2">
         <v>2</v>
       </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>50</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E12">
-        <f>SUM(E6:E11)</f>
+        <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
         <v>29</v>
       </c>
       <c r="F12">
-        <f>SUM(F6:F11)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="G12">
-        <f>SUM(G6:G11)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="H12">
-        <f>SUM(H6:H11)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="I12">
-        <f>SUM(I6:I11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="J12">
-        <f>SUM(J6:J11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K12">
-        <f>SUM(K6:K11)</f>
-        <v>0</v>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="4"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="4"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="7">
+        <f>F12/$E$12</f>
+        <v>0.93103448275862066</v>
+      </c>
+      <c r="J20" s="6">
+        <v>41415</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="7">
+        <f>G12/$E$12</f>
+        <v>0.7931034482758621</v>
+      </c>
+      <c r="J21" s="6">
+        <v>41418</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="7">
+        <f>H12/$E$12</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="J22" s="6">
+        <v>41421</v>
+      </c>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="7">
+        <f>I12/$E$12</f>
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="J23" s="6">
+        <v>41422</v>
+      </c>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="7">
+        <f>J12/$E$12</f>
+        <v>0.20689655172413793</v>
+      </c>
+      <c r="J24" s="6">
+        <v>41423</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="F3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
MAJ des docs - réglement des priorités sprint 2
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -9,25 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint2" sheetId="4" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$A$2:$J$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$2:$K$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$33</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>ITERATION 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>N°</t>
   </si>
@@ -88,6 +86,39 @@
   <si>
     <t>#7</t>
   </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>Changer le type des blocs à poser</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>Régler le problème de poser des blocs sous ou sur soi</t>
+  </si>
+  <si>
+    <t>Enregistrer des macros</t>
+  </si>
+  <si>
+    <t>Rejouer des macros</t>
+  </si>
+  <si>
+    <t>Copier une structure</t>
+  </si>
+  <si>
+    <t>Coller une structure</t>
+  </si>
+  <si>
+    <t>Poser des formes prédéfinies</t>
+  </si>
+  <si>
+    <t>Intégrer la nouvelle implémentation du  joueur</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -159,8 +190,36 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -168,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -186,7 +245,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -292,7 +354,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint1!$J$20:$J$24</c:f>
+              <c:f>Sprint1!$J$17:$J$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -327,7 +389,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint1!$I$20:$I$24</c:f>
+              <c:f>Sprint1!$I$17:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -344,7 +406,7 @@
                   <c:v>0.34482758620689657</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20689655172413793</c:v>
+                  <c:v>6.8965517241379309E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -360,11 +422,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="180812224"/>
-        <c:axId val="180814224"/>
+        <c:axId val="180532640"/>
+        <c:axId val="180551896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180812224"/>
+        <c:axId val="180532640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180814224"/>
+        <c:crossAx val="180551896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -438,7 +500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180814224"/>
+        <c:axId val="180551896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +615,384 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180812224"/>
+        <c:crossAx val="180532640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Evalution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> du RAF pendant le sprint 2(en % )</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint2!$J$16:$J$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31/05/2013</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint2!$I$16:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="180682736"/>
+        <c:axId val="180684216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="180682736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180684216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="180684216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>RAF</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> en %</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180682736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,7 +1081,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1177,6 +2172,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>165884</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1483,10 +2515,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J24"/>
+  <dimension ref="B3:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,28 +2534,28 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="F4" s="6">
         <v>41415</v>
@@ -1543,10 +2575,10 @@
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1572,10 +2604,10 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1596,15 +2628,15 @@
         <v>2</v>
       </c>
       <c r="J6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -1630,10 +2662,10 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1659,10 +2691,10 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1688,10 +2720,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2">
         <v>3</v>
@@ -1712,15 +2744,15 @@
         <v>3</v>
       </c>
       <c r="J10" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -1741,93 +2773,114 @@
         <v>5</v>
       </c>
       <c r="J11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <f t="shared" ref="E12:J12" si="0">SUM(E6:E11)</f>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" ref="E13:J13" si="0">SUM(E6:E11)</f>
         <v>29</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="2"/>
+      <c r="I17" s="7">
+        <f>F13/$E$13</f>
+        <v>0.93103448275862066</v>
+      </c>
+      <c r="J17" s="6">
+        <v>41415</v>
+      </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="4"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="7">
+        <f>G13/$E$13</f>
+        <v>0.7931034482758621</v>
+      </c>
+      <c r="J18" s="6">
+        <v>41418</v>
+      </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="4"/>
-      <c r="J19" s="1"/>
+      <c r="I19" s="7">
+        <f>H13/$E$13</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="J19" s="6">
+        <v>41421</v>
+      </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="7">
-        <f>F12/$E$12</f>
-        <v>0.93103448275862066</v>
+        <f>I13/$E$13</f>
+        <v>0.34482758620689657</v>
       </c>
       <c r="J20" s="6">
-        <v>41415</v>
+        <v>41422</v>
       </c>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" s="7">
-        <f>G12/$E$12</f>
-        <v>0.7931034482758621</v>
+        <f>J13/$E$13</f>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="J21" s="6">
-        <v>41418</v>
-      </c>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="7">
-        <f>H12/$E$12</f>
-        <v>0.55172413793103448</v>
-      </c>
-      <c r="J22" s="6">
-        <v>41421</v>
-      </c>
-    </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="7">
-        <f>I12/$E$12</f>
-        <v>0.34482758620689657</v>
-      </c>
-      <c r="J23" s="6">
-        <v>41422</v>
-      </c>
-    </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I24" s="7">
-        <f>J12/$E$12</f>
-        <v>0.20689655172413793</v>
-      </c>
-      <c r="J24" s="6">
         <v>41423</v>
       </c>
     </row>
@@ -1843,13 +2896,318 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B3:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>41424</v>
+      </c>
+      <c r="G4" s="6">
+        <v>41425</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>SUM(E5:E12)</f>
+        <v>33</v>
+      </c>
+      <c r="F13">
+        <f>SUM(F5:F12)</f>
+        <v>33</v>
+      </c>
+      <c r="G13">
+        <f>SUM(G5:G12)</f>
+        <v>32</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H5:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>SUM(I5:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>SUM(J5:J12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7">
+        <f>F13/$E$13</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
+        <f>F$4</f>
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7">
+        <f>G13/$E$13</f>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="J17" s="6">
+        <f>G4</f>
+        <v>41425</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="7"/>
+      <c r="J20" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MAJ documents avancement et tâches
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$2:$K$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>N°</t>
   </si>
@@ -117,7 +117,13 @@
     <t>Poser des formes prédéfinies</t>
   </si>
   <si>
-    <t>Intégrer la nouvelle implémentation du  joueur</t>
+    <t>Intégrer la nouvelle implémentation du joueur</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>Création du menu</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -422,11 +427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="180532640"/>
-        <c:axId val="180551896"/>
+        <c:axId val="181063104"/>
+        <c:axId val="181065104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180532640"/>
+        <c:axId val="181063104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +463,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -492,7 +496,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180551896"/>
+        <c:crossAx val="181065104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -500,7 +504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180551896"/>
+        <c:axId val="181065104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +555,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -615,7 +618,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180532640"/>
+        <c:crossAx val="181063104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,7 +752,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$J$16:$J$20</c:f>
+              <c:f>Sprint2!$J$17:$J$21</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -757,6 +760,12 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>31/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>03/06/2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>04/06/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -775,7 +784,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint2!$I$16:$I$20</c:f>
+              <c:f>Sprint2!$I$17:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -783,7 +792,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96969696969696972</c:v>
+                  <c:v>0.93023255813953487</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79069767441860461</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69767441860465118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,11 +814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="180682736"/>
-        <c:axId val="180684216"/>
+        <c:axId val="181160584"/>
+        <c:axId val="181222976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="180682736"/>
+        <c:axId val="181160584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +884,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180684216"/>
+        <c:crossAx val="181222976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +892,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180684216"/>
+        <c:axId val="181222976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1007,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180682736"/>
+        <c:crossAx val="181160584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,13 +2209,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>165884</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2899,10 +2914,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J20"/>
+  <dimension ref="B3:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,8 +2962,12 @@
       <c r="G4" s="6">
         <v>41425</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="H4" s="6">
+        <v>41428</v>
+      </c>
+      <c r="I4" s="6">
+        <v>41429</v>
+      </c>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2970,8 +2989,12 @@
       <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -2993,8 +3016,12 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -3016,8 +3043,12 @@
       <c r="G7" s="2">
         <v>6</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6</v>
+      </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -3039,8 +3070,12 @@
       <c r="G8" s="2">
         <v>4</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="2">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -3062,8 +3097,12 @@
       <c r="G9" s="2">
         <v>5</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5</v>
+      </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -3085,8 +3124,12 @@
       <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -3108,8 +3151,12 @@
       <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -3131,75 +3178,116 @@
       <c r="G12" s="2">
         <v>5</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
+      </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <f>SUM(E5:E12)</f>
-        <v>33</v>
-      </c>
-      <c r="F13">
-        <f>SUM(F5:F12)</f>
-        <v>33</v>
-      </c>
-      <c r="G13">
-        <f>SUM(G5:G12)</f>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H13">
-        <f>SUM(H5:H12)</f>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>8</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" ref="E14:J14" si="0">SUM(E5:E13)</f>
+        <v>43</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13">
-        <f>SUM(I5:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f>SUM(J5:J12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I15" s="3" t="s">
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="7">
-        <f>F13/$E$13</f>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7">
+        <f>F14/$E$14</f>
         <v>1</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J17" s="6">
         <f>F$4</f>
         <v>41424</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="7">
-        <f>G13/$E$13</f>
-        <v>0.96969696969696972</v>
-      </c>
-      <c r="J17" s="6">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="7">
+        <f>G14/$E$14</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="J18" s="6">
         <f>G4</f>
         <v>41425</v>
       </c>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="7"/>
-      <c r="J18" s="6"/>
-    </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="7"/>
-      <c r="J19" s="6"/>
+      <c r="I19" s="7">
+        <f>H14/$E$14</f>
+        <v>0.79069767441860461</v>
+      </c>
+      <c r="J19" s="6">
+        <v>41428</v>
+      </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="7"/>
-      <c r="J20" s="6"/>
+      <c r="I20" s="7">
+        <f>I14/$E$14</f>
+        <v>0.69767441860465118</v>
+      </c>
+      <c r="J20" s="6">
+        <v>41429</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="7"/>
+      <c r="J21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mise en place du menu + maj docs (pb retour au jeu)
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$2:$K$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$35</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>N°</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Création du menu</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>Renseigner le joueur avec un HUD (type de bloc,forme…)</t>
   </si>
 </sst>
 </file>
@@ -427,11 +433,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="181063104"/>
-        <c:axId val="181065104"/>
+        <c:axId val="188724600"/>
+        <c:axId val="188789104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181063104"/>
+        <c:axId val="188724600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +502,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181065104"/>
+        <c:crossAx val="188789104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181065104"/>
+        <c:axId val="188789104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +624,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181063104"/>
+        <c:crossAx val="188724600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -752,7 +758,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$J$17:$J$21</c:f>
+              <c:f>Sprint2!$J$18:$J$22</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -766,6 +772,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>04/06/2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>05/06/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -784,7 +793,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint2!$I$17:$I$21</c:f>
+              <c:f>Sprint2!$I$18:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -800,6 +809,9 @@
                 <c:pt idx="3">
                   <c:v>0.69767441860465118</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67441860465116277</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -814,11 +826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="181160584"/>
-        <c:axId val="181222976"/>
+        <c:axId val="188797368"/>
+        <c:axId val="188892760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181160584"/>
+        <c:axId val="188797368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +896,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181222976"/>
+        <c:crossAx val="188892760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -892,7 +904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181222976"/>
+        <c:axId val="188892760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,7 +1019,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181160584"/>
+        <c:crossAx val="188797368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2209,13 +2221,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>165884</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>142070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2914,10 +2926,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J21"/>
+  <dimension ref="B3:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,7 +2980,9 @@
       <c r="I4" s="6">
         <v>41429</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="6">
+        <v>41430</v>
+      </c>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -2995,7 +3009,9 @@
       <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -3022,7 +3038,9 @@
       <c r="I6" s="2">
         <v>0</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -3049,7 +3067,9 @@
       <c r="I7" s="2">
         <v>6</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -3076,7 +3096,9 @@
       <c r="I8" s="2">
         <v>4</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -3103,7 +3125,9 @@
       <c r="I9" s="2">
         <v>5</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -3130,7 +3154,9 @@
       <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -3157,7 +3183,9 @@
       <c r="I11" s="2">
         <v>0</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -3184,7 +3212,9 @@
       <c r="I12" s="2">
         <v>5</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -3211,83 +3241,119 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <f t="shared" ref="E14:J14" si="0">SUM(E5:E13)</f>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>4</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>SUM(E5:E13)</f>
         <v>43</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
+      <c r="F15">
+        <f>SUM(F5:F13)</f>
         <v>43</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+      <c r="G15">
+        <f>SUM(G5:G13)</f>
         <v>40</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
+      <c r="H15">
+        <f>SUM(H5:H13)</f>
         <v>34</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
+      <c r="I15">
+        <f>SUM(I5:I13)</f>
         <v>30</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="3" t="s">
+      <c r="J15">
+        <f>SUM(J5:J13)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="7">
-        <f>F14/$E$14</f>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="7">
+        <f>F15/$E$15</f>
         <v>1</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <f>F$4</f>
         <v>41424</v>
       </c>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="7">
-        <f>G14/$E$14</f>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="7">
+        <f>G15/$E$15</f>
         <v>0.93023255813953487</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J19" s="6">
         <f>G4</f>
         <v>41425</v>
       </c>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="7">
-        <f>H14/$E$14</f>
-        <v>0.79069767441860461</v>
-      </c>
-      <c r="J19" s="6">
-        <v>41428</v>
-      </c>
-    </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="7">
-        <f>I14/$E$14</f>
+        <f>H15/$E$15</f>
+        <v>0.79069767441860461</v>
+      </c>
+      <c r="J20" s="6">
+        <v>41428</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="7">
+        <f>I15/$E$15</f>
         <v>0.69767441860465118</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J21" s="6">
         <v>41429</v>
       </c>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="7"/>
-      <c r="J21" s="6"/>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="7">
+        <f>J15/$E$15</f>
+        <v>0.67441860465116277</v>
+      </c>
+      <c r="J22" s="6">
+        <v>41430</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Maj Docs + Diapo
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Documents\travail\EMN\MiniCraft\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -18,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$2:$K$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$34</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>N°</t>
   </si>
@@ -117,16 +112,10 @@
     <t>Poser des formes prédéfinies</t>
   </si>
   <si>
-    <t>Intégrer la nouvelle implémentation du joueur</t>
-  </si>
-  <si>
     <t>#9</t>
   </si>
   <si>
     <t>Création du menu</t>
-  </si>
-  <si>
-    <t>#10</t>
   </si>
   <si>
     <t>Renseigner le joueur avec un HUD (type de bloc,forme…)</t>
@@ -333,26 +322,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -367,21 +336,9 @@
             <c:strRef>
               <c:f>Sprint1!$J$17:$J$21</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29/05/2013</c:v>
+                  <c:v>21/05/2013 24/05/2013 27/05/2013 28/05/2013 29/05/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -432,12 +389,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="188724600"/>
-        <c:axId val="188789104"/>
+        <c:axId val="69332992"/>
+        <c:axId val="69334912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="188724600"/>
+        <c:axId val="69332992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,32 +435,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188789104"/>
+        <c:crossAx val="69334912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -510,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188789104"/>
+        <c:axId val="69334912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,26 +507,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -624,7 +542,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188724600"/>
+        <c:crossAx val="69332992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -726,26 +644,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -758,23 +656,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$J$18:$J$22</c:f>
+              <c:f>Sprint2!$J$17:$J$22</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31/05/2013</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>03/06/2013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>04/06/2013</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>05/06/2013</c:v>
+                  <c:v>30/05/2013 31/05/2013 03/06/2013 04/06/2013 05/06/2013 07/06/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -793,24 +679,27 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint2!$I$18:$I$22</c:f>
+              <c:f>Sprint2!$I$17:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93023255813953487</c:v>
+                  <c:v>0.92105263157894735</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79069767441860461</c:v>
+                  <c:v>0.76315789473684215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69767441860465118</c:v>
+                  <c:v>0.65789473684210531</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67441860465116277</c:v>
+                  <c:v>0.63157894736842102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26315789473684209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,12 +714,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="188797368"/>
-        <c:axId val="188892760"/>
+        <c:axId val="40634624"/>
+        <c:axId val="40661376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="188797368"/>
+        <c:axId val="40634624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,32 +761,12 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188892760"/>
+        <c:crossAx val="40661376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -904,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188892760"/>
+        <c:axId val="40661376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,26 +834,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1019,7 +869,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188797368"/>
+        <c:crossAx val="40634624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2221,13 +2071,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>165884</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2295,7 +2145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2330,7 +2180,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2926,10 +2776,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:J22"/>
+  <dimension ref="B3:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2943,7 +2793,7 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2955,7 +2805,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2983,8 +2833,11 @@
       <c r="J4" s="6">
         <v>41430</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="6">
+        <v>41432</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3012,8 +2865,11 @@
       <c r="J5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3041,8 +2897,11 @@
       <c r="J6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3070,8 +2929,11 @@
       <c r="J7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -3099,8 +2961,11 @@
       <c r="J8" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -3128,8 +2993,11 @@
       <c r="J9" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -3157,8 +3025,11 @@
       <c r="J10" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -3186,25 +3057,28 @@
       <c r="J11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H12" s="2">
         <v>5</v>
@@ -3213,12 +3087,15 @@
         <v>5</v>
       </c>
       <c r="J12" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -3227,132 +3104,119 @@
         <v>2</v>
       </c>
       <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>SUM(E5:E12)</f>
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <f>SUM(F5:F12)</f>
+        <v>38</v>
+      </c>
+      <c r="G14">
+        <f>SUM(G5:G12)</f>
+        <v>35</v>
+      </c>
+      <c r="H14">
+        <f>SUM(H5:H12)</f>
+        <v>29</v>
+      </c>
+      <c r="I14">
+        <f>SUM(I5:I12)</f>
+        <v>25</v>
+      </c>
+      <c r="J14">
+        <f>SUM(J5:J12)</f>
+        <v>24</v>
+      </c>
+      <c r="K14">
+        <f>SUM(K5:K12)</f>
         <v>10</v>
       </c>
-      <c r="F13" s="2">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2">
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="I13" s="2">
-        <v>5</v>
-      </c>
-      <c r="J13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2">
-        <v>4</v>
-      </c>
-      <c r="I14" s="2">
-        <v>3</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7">
+        <f>F14/$E$14</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <f>SUM(E5:E13)</f>
-        <v>43</v>
-      </c>
-      <c r="F15">
-        <f>SUM(F5:F13)</f>
-        <v>43</v>
-      </c>
-      <c r="G15">
-        <f>SUM(G5:G13)</f>
-        <v>40</v>
-      </c>
-      <c r="H15">
-        <f>SUM(H5:H13)</f>
-        <v>34</v>
-      </c>
-      <c r="I15">
-        <f>SUM(I5:I13)</f>
-        <v>30</v>
-      </c>
-      <c r="J15">
-        <f>SUM(J5:J13)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>23</v>
+      <c r="J17" s="6">
+        <f>F$4</f>
+        <v>41424</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="7">
-        <f>F15/$E$15</f>
-        <v>1</v>
+        <f>G14/$E$14</f>
+        <v>0.92105263157894735</v>
       </c>
       <c r="J18" s="6">
-        <f>F$4</f>
-        <v>41424</v>
+        <f>G4</f>
+        <v>41425</v>
       </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I19" s="7">
-        <f>G15/$E$15</f>
-        <v>0.93023255813953487</v>
+        <f>H14/$E$14</f>
+        <v>0.76315789473684215</v>
       </c>
       <c r="J19" s="6">
-        <f>G4</f>
-        <v>41425</v>
+        <v>41428</v>
       </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="7">
-        <f>H15/$E$15</f>
-        <v>0.79069767441860461</v>
+        <f>I14/$E$14</f>
+        <v>0.65789473684210531</v>
       </c>
       <c r="J20" s="6">
-        <v>41428</v>
+        <v>41429</v>
       </c>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" s="7">
-        <f>I15/$E$15</f>
-        <v>0.69767441860465118</v>
+        <f>J14/$E$14</f>
+        <v>0.63157894736842102</v>
       </c>
       <c r="J21" s="6">
-        <v>41429</v>
+        <v>41430</v>
       </c>
     </row>
     <row r="22" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I22" s="7">
-        <f>J15/$E$15</f>
-        <v>0.67441860465116277</v>
+        <f>K14/$E$14</f>
+        <v>0.26315789473684209</v>
       </c>
       <c r="J22" s="6">
-        <v>41430</v>
+        <v>41432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour docs pré-soutenance
</commit_message>
<xml_diff>
--- a/doc/Agile.xlsx
+++ b/doc/Agile.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Documents\travail\EMN\MiniCraft\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$2:$K$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sprint2!$B$2:$K$34</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -228,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -252,6 +257,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,6 +322,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -322,6 +331,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -336,9 +365,21 @@
             <c:strRef>
               <c:f>Sprint1!$J$17:$J$21</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>21/05/2013 24/05/2013 27/05/2013 28/05/2013 29/05/2013</c:v>
+                  <c:v>21/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28/05/2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29/05/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -389,13 +430,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69332992"/>
-        <c:axId val="69334912"/>
+        <c:axId val="179616192"/>
+        <c:axId val="179641312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69332992"/>
+        <c:axId val="179616192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,6 +467,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -435,12 +476,32 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69334912"/>
+        <c:crossAx val="179641312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -448,7 +509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69334912"/>
+        <c:axId val="179641312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,6 +560,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -507,6 +569,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -542,7 +624,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69332992"/>
+        <c:crossAx val="179616192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -644,6 +726,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -656,11 +758,35 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint2!$J$17:$J$22</c:f>
+              <c:f>Sprint2!$J$17:$J$26</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>30/05/2013 31/05/2013 03/06/2013 04/06/2013 05/06/2013 07/06/2013</c:v>
+                  <c:v>5/30/2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5/31/2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6/3/2013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6/4/2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6/5/2013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6/7/2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6/8/2013</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6/9/2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6/12/2013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -679,27 +805,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sprint2!$I$17:$I$22</c:f>
+              <c:f>Sprint2!$I$17:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92105263157894735</c:v>
+                  <c:v>0.92500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76315789473684215</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65789473684210531</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63157894736842102</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26315789473684209</c:v>
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,13 +849,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40634624"/>
-        <c:axId val="40661376"/>
+        <c:axId val="158543472"/>
+        <c:axId val="179729704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40634624"/>
+        <c:axId val="158543472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,12 +895,32 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40661376"/>
+        <c:crossAx val="179729704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40661376"/>
+        <c:axId val="179729704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,6 +988,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -869,7 +1043,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40634624"/>
+        <c:crossAx val="158543472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2145,7 +2319,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2180,7 +2354,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2394,7 +2568,7 @@
   </sheetPr>
   <dimension ref="B3:J21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -2776,10 +2950,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:K22"/>
+  <dimension ref="B3:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,19 +2967,19 @@
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2836,8 +3010,17 @@
       <c r="K4" s="6">
         <v>41432</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="6">
+        <v>41433</v>
+      </c>
+      <c r="M4" s="6">
+        <v>41434</v>
+      </c>
+      <c r="N4" s="6">
+        <v>41437</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2868,8 +3051,17 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2900,8 +3092,17 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2912,28 +3113,37 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2">
         <v>6</v>
       </c>
       <c r="J7" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2962,10 +3172,19 @@
         <v>4</v>
       </c>
       <c r="K8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -2996,8 +3215,17 @@
       <c r="K9" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -3028,8 +3256,17 @@
       <c r="K10" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="2">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -3049,10 +3286,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
@@ -3060,8 +3297,17 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -3081,19 +3327,28 @@
         <v>8</v>
       </c>
       <c r="H12" s="2">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2">
+        <v>6</v>
+      </c>
+      <c r="K12" s="2">
         <v>5</v>
       </c>
-      <c r="I12" s="2">
-        <v>5</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="L12" s="2">
         <v>4</v>
       </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
@@ -3116,46 +3371,67 @@
         <v>4</v>
       </c>
       <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2">
         <v>3</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
         <v>1</v>
       </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E14">
-        <f>SUM(E5:E12)</f>
-        <v>38</v>
+        <f t="shared" ref="E14:K14" si="0">SUM(E5:E12)</f>
+        <v>40</v>
       </c>
       <c r="F14">
-        <f>SUM(F5:F12)</f>
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="G14">
-        <f>SUM(G5:G12)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="H14">
-        <f>SUM(H5:H12)</f>
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="I14">
-        <f>SUM(I5:I12)</f>
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="J14">
-        <f>SUM(J5:J12)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="K14">
-        <f>SUM(K5:K12)</f>
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:M14" si="1">SUM(L5:L12)</f>
+        <v>18</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14" si="2">SUM(N5:N12)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I16" s="3" t="s">
         <v>8</v>
       </c>
@@ -3176,7 +3452,7 @@
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="7">
         <f>G14/$E$14</f>
-        <v>0.92105263157894735</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="J18" s="6">
         <f>G4</f>
@@ -3186,7 +3462,7 @@
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I19" s="7">
         <f>H14/$E$14</f>
-        <v>0.76315789473684215</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="J19" s="6">
         <v>41428</v>
@@ -3195,7 +3471,7 @@
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="7">
         <f>I14/$E$14</f>
-        <v>0.65789473684210531</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="J20" s="6">
         <v>41429</v>
@@ -3204,7 +3480,7 @@
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I21" s="7">
         <f>J14/$E$14</f>
-        <v>0.63157894736842102</v>
+        <v>0.6</v>
       </c>
       <c r="J21" s="6">
         <v>41430</v>
@@ -3213,16 +3489,40 @@
     <row r="22" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I22" s="7">
         <f>K14/$E$14</f>
-        <v>0.26315789473684209</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J22" s="6">
         <v>41432</v>
       </c>
     </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="7">
+        <f>L14/$E$14</f>
+        <v>0.45</v>
+      </c>
+      <c r="J23" s="6">
+        <v>41433</v>
+      </c>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="7">
+        <f>M14/$E$14</f>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="J24" s="6">
+        <v>41434</v>
+      </c>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="7">
+        <f>N14/$E$14</f>
+        <v>0.25</v>
+      </c>
+      <c r="J25" s="6">
+        <v>41437</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F3:J3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>